<commit_message>
Filled dbconcept with example data
</commit_message>
<xml_diff>
--- a/DBConcept.xlsx
+++ b/DBConcept.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Cooldown</t>
   </si>
   <si>
-    <t>Unit Type</t>
-  </si>
-  <si>
     <t>AtkType ID</t>
   </si>
   <si>
@@ -115,6 +112,87 @@
   </si>
   <si>
     <t>Hoero ID</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Melee</t>
+  </si>
+  <si>
+    <t>Ranged</t>
+  </si>
+  <si>
+    <t>Siege</t>
+  </si>
+  <si>
+    <t>Aerial</t>
+  </si>
+  <si>
+    <t>Evil</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Demigod</t>
+  </si>
+  <si>
+    <t>Mythical</t>
+  </si>
+  <si>
+    <t>Magical</t>
+  </si>
+  <si>
+    <t>Rain of Fire</t>
+  </si>
+  <si>
+    <t>Barrage</t>
+  </si>
+  <si>
+    <t>Headbutt</t>
+  </si>
+  <si>
+    <t>Bombardment</t>
+  </si>
+  <si>
+    <t>Forceful Slash</t>
+  </si>
+  <si>
+    <t>Unit Name</t>
+  </si>
+  <si>
+    <t>Elven Archer</t>
+  </si>
+  <si>
+    <t>Shieldmaiden</t>
+  </si>
+  <si>
+    <t>Pegasus</t>
+  </si>
+  <si>
+    <t>Pixie</t>
+  </si>
+  <si>
+    <t>Bron</t>
+  </si>
+  <si>
+    <t>Swordsman</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>dmg/sec</t>
+  </si>
+  <si>
+    <t>300*45</t>
+  </si>
+  <si>
+    <t>300*(20/2.4)</t>
   </si>
 </sst>
 </file>
@@ -186,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -229,11 +307,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -266,45 +353,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD27"/>
+  <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,108 +751,111 @@
     <col min="28" max="28" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="15"/>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="Y1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="Y1" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="15"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
       <c r="P2" s="15"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21"/>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="21"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30"/>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
+      <c r="AE2" s="30"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17" t="s">
+      <c r="J3" s="21"/>
+      <c r="K3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="17"/>
+      <c r="L3" s="21"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="Q3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="R3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
       <c r="U3" s="2" t="s">
         <v>5</v>
       </c>
@@ -772,266 +865,415 @@
       <c r="Y3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Z3" s="17" t="s">
+      <c r="Z3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="12" t="s">
         <v>7</v>
-      </c>
-      <c r="AA3" s="17"/>
-      <c r="AB3" s="12" t="s">
-        <v>8</v>
       </c>
       <c r="AC3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="17"/>
-      <c r="AA4" s="17"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="17"/>
-      <c r="AA5" s="17"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="17"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="17"/>
-      <c r="AA7" s="17"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="17"/>
-      <c r="AA8" s="17"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+        <v>8</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>1</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="I4" s="21">
+        <v>1</v>
+      </c>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="21"/>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="1">
+        <v>200</v>
+      </c>
+      <c r="V4" s="1">
+        <v>30</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="13">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>15</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>2</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="I5" s="21">
+        <v>2</v>
+      </c>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="Q5" s="1">
+        <v>2</v>
+      </c>
+      <c r="R5" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="1">
+        <v>300</v>
+      </c>
+      <c r="V5" s="1">
+        <v>40</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
+        <v>3</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="I6" s="21">
+        <v>3</v>
+      </c>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="Q6" s="1">
+        <v>3</v>
+      </c>
+      <c r="R6" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="1">
+        <v>400</v>
+      </c>
+      <c r="V6" s="1">
+        <v>50</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="13">
+        <v>4</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>20</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>4</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="I7" s="21">
+        <v>4</v>
+      </c>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="21"/>
+      <c r="Q7" s="1">
+        <v>4</v>
+      </c>
+      <c r="R7" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="1">
+        <v>500</v>
+      </c>
+      <c r="V7" s="1">
+        <v>60</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="13">
+        <v>5</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>15</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>5</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="I8" s="21">
+        <v>5</v>
+      </c>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="21"/>
+      <c r="Q8" s="1">
+        <v>5</v>
+      </c>
+      <c r="R8" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="1">
+        <v>600</v>
+      </c>
+      <c r="V8" s="1">
+        <v>70</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z8" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>10</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="17"/>
-      <c r="AA9" s="17"/>
+      <c r="Z9" s="21"/>
+      <c r="AA9" s="21"/>
       <c r="AB9" s="13"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
+      <c r="AE9" s="1"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
       <c r="H14" s="15"/>
-      <c r="I14" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
+      <c r="I14" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
       <c r="Q14" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
       <c r="T14" s="20"/>
       <c r="U14" s="20"/>
       <c r="V14" s="20"/>
-      <c r="Y14" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="23"/>
-      <c r="AB14" s="23"/>
-      <c r="AC14" s="23"/>
-      <c r="AD14" s="23"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
+      <c r="Y14" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="24"/>
+      <c r="AD14" s="24"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
       <c r="T15" s="20"/>
       <c r="U15" s="20"/>
       <c r="V15" s="20"/>
-      <c r="Y15" s="23"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="23"/>
-      <c r="AC15" s="23"/>
-      <c r="AD15" s="23"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="Y15" s="24"/>
+      <c r="Z15" s="24"/>
+      <c r="AA15" s="24"/>
+      <c r="AB15" s="24"/>
+      <c r="AC15" s="24"/>
+      <c r="AD15" s="24"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17" t="s">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="15"/>
       <c r="I16" s="14" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="14" t="s">
         <v>16</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>17</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R16" s="17" t="s">
+      <c r="R16" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="S16" s="17"/>
-      <c r="T16" s="17"/>
-      <c r="U16" s="4" t="s">
+      <c r="V16" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="V16" s="10" t="s">
-        <v>13</v>
       </c>
       <c r="Y16" s="3" t="s">
         <v>0</v>
@@ -1040,253 +1282,297 @@
         <v>2</v>
       </c>
       <c r="AA16" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC16" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD16" s="17"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
+        <v>11</v>
+      </c>
+      <c r="AC16" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD16" s="21"/>
+      <c r="AE16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
         <v>1</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
       <c r="I17" s="14">
         <v>1</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="29">
+        <v>20</v>
+      </c>
+      <c r="K17" s="18">
         <v>2</v>
       </c>
       <c r="L17" s="14">
         <v>1000</v>
       </c>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="11"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="9"/>
-      <c r="AA17" s="7"/>
-      <c r="AB17" s="5"/>
-      <c r="AC17" s="17"/>
-      <c r="AD17" s="17"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+      <c r="Q17" s="1">
+        <v>1</v>
+      </c>
+      <c r="R17" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="5">
+        <v>5</v>
+      </c>
+      <c r="V17" s="11">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="9">
         <v>2</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
+      <c r="AA17" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC17" s="21">
+        <v>300</v>
+      </c>
+      <c r="AD17" s="21"/>
+      <c r="AE17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <v>2</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
       <c r="I18" s="14">
         <v>2</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" s="29">
+        <v>21</v>
+      </c>
+      <c r="K18" s="18">
         <v>1</v>
       </c>
       <c r="L18" s="14">
         <v>10000</v>
       </c>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
+      <c r="Q18" s="1">
+        <v>2</v>
+      </c>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
       <c r="U18" s="5"/>
       <c r="V18" s="11"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="9"/>
       <c r="AA18" s="7"/>
       <c r="AB18" s="5"/>
-      <c r="AC18" s="17"/>
-      <c r="AD18" s="17"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC18" s="21"/>
+      <c r="AD18" s="21"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
-      <c r="K19" s="29"/>
+      <c r="K19" s="18"/>
       <c r="L19" s="14"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
+      <c r="Q19" s="1">
+        <v>3</v>
+      </c>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
       <c r="U19" s="5"/>
       <c r="V19" s="11"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="9"/>
       <c r="AA19" s="7"/>
       <c r="AB19" s="5"/>
-      <c r="AC19" s="17"/>
-      <c r="AD19" s="17"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC19" s="21"/>
+      <c r="AD19" s="21"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
-      <c r="K20" s="29"/>
+      <c r="K20" s="18"/>
       <c r="L20" s="14"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
+      <c r="Q20" s="1">
+        <v>4</v>
+      </c>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
       <c r="U20" s="5"/>
       <c r="V20" s="11"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="9"/>
       <c r="AA20" s="7"/>
       <c r="AB20" s="5"/>
-      <c r="AC20" s="17"/>
-      <c r="AD20" s="17"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
+      <c r="AC20" s="21"/>
+      <c r="AD20" s="21"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
-      <c r="K21" s="29"/>
+      <c r="K21" s="18"/>
       <c r="L21" s="14"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
       <c r="U21" s="5"/>
       <c r="V21" s="11"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="9"/>
       <c r="AA21" s="7"/>
       <c r="AB21" s="5"/>
-      <c r="AC21" s="17"/>
-      <c r="AD21" s="17"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+      <c r="AC21" s="21"/>
+      <c r="AD21" s="21"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-      <c r="K22" s="29"/>
+      <c r="K22" s="18"/>
       <c r="L22" s="14"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
       <c r="U22" s="5"/>
       <c r="V22" s="11"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="9"/>
       <c r="AA22" s="7"/>
       <c r="AB22" s="5"/>
-      <c r="AC22" s="17"/>
-      <c r="AD22" s="17"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC22" s="21"/>
+      <c r="AD22" s="21"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
-      <c r="K23" s="29"/>
+      <c r="K23" s="18"/>
       <c r="L23" s="14"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
       <c r="U23" s="5"/>
       <c r="V23" s="11"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="9"/>
       <c r="AA23" s="7"/>
       <c r="AB23" s="5"/>
-      <c r="AC23" s="17"/>
-      <c r="AD23" s="17"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC23" s="21"/>
+      <c r="AD23" s="21"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="27"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B24" s="7">
+        <v>1</v>
+      </c>
+      <c r="C24" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="7"/>
-      <c r="C25" s="27"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C25" s="17"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="7"/>
-      <c r="C26" s="27"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C26" s="17"/>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="7"/>
-      <c r="C27" s="27"/>
+      <c r="C27" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="A21:C22"/>
-    <mergeCell ref="Q14:V15"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="I14:L15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A14:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="AC22:AD22"/>
-    <mergeCell ref="AC23:AD23"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="AC20:AD20"/>
-    <mergeCell ref="AC21:AD21"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="Y14:AD15"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AC18:AD18"/>
-    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="Y1:AE2"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="I1:O2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D8:F8"/>
     <mergeCell ref="R8:T8"/>
     <mergeCell ref="R9:T9"/>
-    <mergeCell ref="Y1:AD2"/>
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="Z5:AA5"/>
@@ -1300,37 +1586,33 @@
     <mergeCell ref="R5:T5"/>
     <mergeCell ref="R6:T6"/>
     <mergeCell ref="R7:T7"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="I1:O2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="Y14:AD15"/>
+    <mergeCell ref="AC16:AD16"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="AC20:AD20"/>
+    <mergeCell ref="AC21:AD21"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="AC22:AD22"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="A21:C22"/>
+    <mergeCell ref="Q14:V15"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="I14:L15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A14:G15"/>
+    <mergeCell ref="D16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Applied temporary fixes so that the db may create each time
</commit_message>
<xml_diff>
--- a/DBConcept.xlsx
+++ b/DBConcept.xlsx
@@ -360,45 +360,45 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -439,9 +439,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office тема">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Оffice">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -479,7 +479,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Оffice">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -551,7 +551,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Оffice">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AF9" sqref="AF9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,25 +755,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="15"/>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
       <c r="P1" s="15"/>
       <c r="Q1" s="25" t="s">
         <v>3</v>
@@ -783,32 +783,32 @@
       <c r="T1" s="25"/>
       <c r="U1" s="25"/>
       <c r="V1" s="25"/>
-      <c r="Y1" s="29" t="s">
+      <c r="Y1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="15"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="25"/>
       <c r="R2" s="25"/>
@@ -816,46 +816,46 @@
       <c r="T2" s="25"/>
       <c r="U2" s="25"/>
       <c r="V2" s="25"/>
-      <c r="Y2" s="29"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21" t="s">
+      <c r="J3" s="22"/>
+      <c r="K3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="21"/>
+      <c r="L3" s="22"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="Q3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
       <c r="U3" s="2" t="s">
         <v>5</v>
       </c>
@@ -865,10 +865,10 @@
       <c r="Y3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Z3" s="21" t="s">
+      <c r="Z3" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="AA3" s="21"/>
+      <c r="AA3" s="22"/>
       <c r="AB3" s="12" t="s">
         <v>7</v>
       </c>
@@ -883,32 +883,32 @@
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="A4" s="22">
         <v>1</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="I4" s="21">
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="I4" s="22">
         <v>1</v>
       </c>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21" t="s">
+      <c r="J4" s="22"/>
+      <c r="K4" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="21"/>
+      <c r="L4" s="22"/>
       <c r="Q4" s="1">
         <v>1</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="R4" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
       <c r="U4" s="1">
         <v>200</v>
       </c>
@@ -918,10 +918,10 @@
       <c r="Y4" s="1">
         <v>1</v>
       </c>
-      <c r="Z4" s="21" t="s">
+      <c r="Z4" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="21"/>
+      <c r="AA4" s="22"/>
       <c r="AB4" s="13">
         <v>2</v>
       </c>
@@ -936,32 +936,32 @@
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="A5" s="22">
         <v>2</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="I5" s="21">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="I5" s="22">
         <v>2</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21" t="s">
+      <c r="J5" s="22"/>
+      <c r="K5" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="21"/>
+      <c r="L5" s="22"/>
       <c r="Q5" s="1">
         <v>2</v>
       </c>
-      <c r="R5" s="21" t="s">
+      <c r="R5" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
       <c r="U5" s="1">
         <v>300</v>
       </c>
@@ -971,10 +971,10 @@
       <c r="Y5" s="1">
         <v>2</v>
       </c>
-      <c r="Z5" s="21" t="s">
+      <c r="Z5" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="AA5" s="21"/>
+      <c r="AA5" s="22"/>
       <c r="AB5" s="13">
         <v>1</v>
       </c>
@@ -989,32 +989,32 @@
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
+      <c r="A6" s="22">
         <v>3</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="I6" s="21">
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="I6" s="22">
         <v>3</v>
       </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21" t="s">
+      <c r="J6" s="22"/>
+      <c r="K6" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="21"/>
+      <c r="L6" s="22"/>
       <c r="Q6" s="1">
         <v>3</v>
       </c>
-      <c r="R6" s="21" t="s">
+      <c r="R6" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
       <c r="U6" s="1">
         <v>400</v>
       </c>
@@ -1024,10 +1024,10 @@
       <c r="Y6" s="1">
         <v>3</v>
       </c>
-      <c r="Z6" s="21" t="s">
+      <c r="Z6" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="AA6" s="21"/>
+      <c r="AA6" s="22"/>
       <c r="AB6" s="13">
         <v>4</v>
       </c>
@@ -1042,32 +1042,32 @@
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="A7" s="22">
         <v>4</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="I7" s="21">
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="I7" s="22">
         <v>4</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21" t="s">
+      <c r="J7" s="22"/>
+      <c r="K7" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="21"/>
+      <c r="L7" s="22"/>
       <c r="Q7" s="1">
         <v>4</v>
       </c>
-      <c r="R7" s="21" t="s">
+      <c r="R7" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
       <c r="U7" s="1">
         <v>500</v>
       </c>
@@ -1077,10 +1077,10 @@
       <c r="Y7" s="1">
         <v>4</v>
       </c>
-      <c r="Z7" s="21" t="s">
+      <c r="Z7" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AA7" s="21"/>
+      <c r="AA7" s="22"/>
       <c r="AB7" s="13">
         <v>5</v>
       </c>
@@ -1095,32 +1095,32 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="22">
         <v>5</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="I8" s="21">
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="I8" s="22">
         <v>5</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21" t="s">
+      <c r="J8" s="22"/>
+      <c r="K8" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="21"/>
+      <c r="L8" s="22"/>
       <c r="Q8" s="1">
         <v>5</v>
       </c>
-      <c r="R8" s="21" t="s">
+      <c r="R8" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
       <c r="U8" s="1">
         <v>600</v>
       </c>
@@ -1130,10 +1130,10 @@
       <c r="Y8" s="1">
         <v>5</v>
       </c>
-      <c r="Z8" s="21" t="s">
+      <c r="Z8" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AA8" s="21"/>
+      <c r="AA8" s="22"/>
       <c r="AB8" s="13">
         <v>1</v>
       </c>
@@ -1148,106 +1148,106 @@
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
       <c r="AB9" s="13"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
       <c r="H14" s="15"/>
-      <c r="I14" s="22" t="s">
+      <c r="I14" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="Q14" s="20" t="s">
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="Q14" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="20"/>
-      <c r="V14" s="20"/>
-      <c r="Y14" s="24" t="s">
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="Y14" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="Z14" s="24"/>
-      <c r="AA14" s="24"/>
-      <c r="AB14" s="24"/>
-      <c r="AC14" s="24"/>
-      <c r="AD14" s="24"/>
+      <c r="Z14" s="26"/>
+      <c r="AA14" s="26"/>
+      <c r="AB14" s="26"/>
+      <c r="AC14" s="26"/>
+      <c r="AD14" s="26"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="20"/>
-      <c r="U15" s="20"/>
-      <c r="V15" s="20"/>
-      <c r="Y15" s="24"/>
-      <c r="Z15" s="24"/>
-      <c r="AA15" s="24"/>
-      <c r="AB15" s="24"/>
-      <c r="AC15" s="24"/>
-      <c r="AD15" s="24"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="15"/>
       <c r="I16" s="14" t="s">
         <v>0</v>
@@ -1264,11 +1264,11 @@
       <c r="Q16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R16" s="21" t="s">
+      <c r="R16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
       <c r="U16" s="4" t="s">
         <v>11</v>
       </c>
@@ -1287,10 +1287,10 @@
       <c r="AB16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AC16" s="21" t="s">
+      <c r="AC16" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="AD16" s="21"/>
+      <c r="AD16" s="22"/>
       <c r="AE16" t="s">
         <v>54</v>
       </c>
@@ -1299,16 +1299,16 @@
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="22">
         <v>1</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
       <c r="I17" s="14">
         <v>1</v>
       </c>
@@ -1324,11 +1324,11 @@
       <c r="Q17" s="1">
         <v>1</v>
       </c>
-      <c r="R17" s="21" t="s">
+      <c r="R17" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
       <c r="U17" s="5">
         <v>5</v>
       </c>
@@ -1347,10 +1347,10 @@
       <c r="AB17" s="5">
         <v>4</v>
       </c>
-      <c r="AC17" s="21">
+      <c r="AC17" s="22">
         <v>300</v>
       </c>
-      <c r="AD17" s="21"/>
+      <c r="AD17" s="22"/>
       <c r="AE17" t="s">
         <v>56</v>
       </c>
@@ -1359,16 +1359,16 @@
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+      <c r="A18" s="22">
         <v>2</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21" t="s">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
       <c r="I18" s="14">
         <v>2</v>
       </c>
@@ -1384,17 +1384,17 @@
       <c r="Q18" s="1">
         <v>2</v>
       </c>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
       <c r="U18" s="5"/>
       <c r="V18" s="11"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="9"/>
       <c r="AA18" s="7"/>
       <c r="AB18" s="5"/>
-      <c r="AC18" s="21"/>
-      <c r="AD18" s="21"/>
+      <c r="AC18" s="22"/>
+      <c r="AD18" s="22"/>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I19" s="14"/>
@@ -1404,17 +1404,17 @@
       <c r="Q19" s="1">
         <v>3</v>
       </c>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
       <c r="U19" s="5"/>
       <c r="V19" s="11"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="9"/>
       <c r="AA19" s="7"/>
       <c r="AB19" s="5"/>
-      <c r="AC19" s="21"/>
-      <c r="AD19" s="21"/>
+      <c r="AC19" s="22"/>
+      <c r="AD19" s="22"/>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I20" s="14"/>
@@ -1424,24 +1424,24 @@
       <c r="Q20" s="1">
         <v>4</v>
       </c>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
       <c r="U20" s="5"/>
       <c r="V20" s="11"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="9"/>
       <c r="AA20" s="7"/>
       <c r="AB20" s="5"/>
-      <c r="AC20" s="21"/>
-      <c r="AD20" s="21"/>
+      <c r="AC20" s="22"/>
+      <c r="AD20" s="22"/>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -1450,22 +1450,22 @@
       <c r="K21" s="18"/>
       <c r="L21" s="14"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
       <c r="U21" s="5"/>
       <c r="V21" s="11"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="9"/>
       <c r="AA21" s="7"/>
       <c r="AB21" s="5"/>
-      <c r="AC21" s="21"/>
-      <c r="AD21" s="21"/>
+      <c r="AC21" s="22"/>
+      <c r="AD21" s="22"/>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
@@ -1474,17 +1474,17 @@
       <c r="K22" s="18"/>
       <c r="L22" s="14"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
       <c r="U22" s="5"/>
       <c r="V22" s="11"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="9"/>
       <c r="AA22" s="7"/>
       <c r="AB22" s="5"/>
-      <c r="AC22" s="21"/>
-      <c r="AD22" s="21"/>
+      <c r="AC22" s="22"/>
+      <c r="AD22" s="22"/>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1501,17 +1501,17 @@
       <c r="K23" s="18"/>
       <c r="L23" s="14"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="21"/>
-      <c r="S23" s="21"/>
-      <c r="T23" s="21"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="22"/>
       <c r="U23" s="5"/>
       <c r="V23" s="11"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="9"/>
       <c r="AA23" s="7"/>
       <c r="AB23" s="5"/>
-      <c r="AC23" s="21"/>
-      <c r="AD23" s="21"/>
+      <c r="AC23" s="22"/>
+      <c r="AD23" s="22"/>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
@@ -1539,13 +1539,59 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="Y1:AE2"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="I1:O2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A21:C22"/>
+    <mergeCell ref="Q14:V15"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="I14:L15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A14:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="AC22:AD22"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="AC20:AD20"/>
+    <mergeCell ref="AC21:AD21"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="Y14:AD15"/>
+    <mergeCell ref="AC16:AD16"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="Z9:AA9"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="K5:L5"/>
@@ -1559,60 +1605,14 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="I9:J9"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="Z8:AA8"/>
-    <mergeCell ref="Z9:AA9"/>
+    <mergeCell ref="Y1:AE2"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="I1:O2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="Q1:V2"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="Y14:AD15"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AC18:AD18"/>
-    <mergeCell ref="AC19:AD19"/>
-    <mergeCell ref="AC20:AD20"/>
-    <mergeCell ref="AC21:AD21"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="AC22:AD22"/>
-    <mergeCell ref="AC23:AD23"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="A21:C22"/>
-    <mergeCell ref="Q14:V15"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="I14:L15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A14:G15"/>
-    <mergeCell ref="D16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Created generator for the zipped reports
</commit_message>
<xml_diff>
--- a/DBConcept.xlsx
+++ b/DBConcept.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="480" yWindow="165" windowWidth="20730" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -360,6 +360,27 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -369,36 +390,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -439,9 +439,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office тема">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Оffice">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -479,7 +479,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Оffice">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -551,7 +551,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Оffice">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AF9" sqref="AF9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Z6" sqref="Z6:AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,107 +755,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
       <c r="H1" s="15"/>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
       <c r="P1" s="15"/>
-      <c r="Q1" s="25" t="s">
+      <c r="Q1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="Y1" s="19" t="s">
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="Y1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
       <c r="H2" s="15"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
       <c r="P2" s="15"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22" t="s">
+      <c r="J3" s="21"/>
+      <c r="K3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="22"/>
+      <c r="L3" s="21"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="Q3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="22" t="s">
+      <c r="R3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
       <c r="U3" s="2" t="s">
         <v>5</v>
       </c>
@@ -865,10 +865,10 @@
       <c r="Y3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Z3" s="22" t="s">
+      <c r="Z3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="AA3" s="22"/>
+      <c r="AA3" s="21"/>
       <c r="AB3" s="12" t="s">
         <v>7</v>
       </c>
@@ -883,32 +883,32 @@
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+      <c r="A4" s="21">
         <v>1</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="I4" s="22">
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="I4" s="21">
         <v>1</v>
       </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22" t="s">
+      <c r="J4" s="21"/>
+      <c r="K4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="22"/>
+      <c r="L4" s="21"/>
       <c r="Q4" s="1">
         <v>1</v>
       </c>
-      <c r="R4" s="22" t="s">
+      <c r="R4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
       <c r="U4" s="1">
         <v>200</v>
       </c>
@@ -918,10 +918,10 @@
       <c r="Y4" s="1">
         <v>1</v>
       </c>
-      <c r="Z4" s="22" t="s">
+      <c r="Z4" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="22"/>
+      <c r="AA4" s="21"/>
       <c r="AB4" s="13">
         <v>2</v>
       </c>
@@ -936,32 +936,32 @@
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>2</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="I5" s="22">
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="I5" s="21">
         <v>2</v>
       </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22" t="s">
+      <c r="J5" s="21"/>
+      <c r="K5" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="22"/>
+      <c r="L5" s="21"/>
       <c r="Q5" s="1">
         <v>2</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="R5" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
       <c r="U5" s="1">
         <v>300</v>
       </c>
@@ -971,10 +971,10 @@
       <c r="Y5" s="1">
         <v>2</v>
       </c>
-      <c r="Z5" s="22" t="s">
+      <c r="Z5" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="AA5" s="22"/>
+      <c r="AA5" s="21"/>
       <c r="AB5" s="13">
         <v>1</v>
       </c>
@@ -989,32 +989,32 @@
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>3</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="I6" s="22">
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="I6" s="21">
         <v>3</v>
       </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22" t="s">
+      <c r="J6" s="21"/>
+      <c r="K6" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="22"/>
+      <c r="L6" s="21"/>
       <c r="Q6" s="1">
         <v>3</v>
       </c>
-      <c r="R6" s="22" t="s">
+      <c r="R6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
       <c r="U6" s="1">
         <v>400</v>
       </c>
@@ -1024,10 +1024,10 @@
       <c r="Y6" s="1">
         <v>3</v>
       </c>
-      <c r="Z6" s="22" t="s">
+      <c r="Z6" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="AA6" s="22"/>
+      <c r="AA6" s="21"/>
       <c r="AB6" s="13">
         <v>4</v>
       </c>
@@ -1042,32 +1042,32 @@
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="21">
         <v>4</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="I7" s="22">
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="I7" s="21">
         <v>4</v>
       </c>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22" t="s">
+      <c r="J7" s="21"/>
+      <c r="K7" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="22"/>
+      <c r="L7" s="21"/>
       <c r="Q7" s="1">
         <v>4</v>
       </c>
-      <c r="R7" s="22" t="s">
+      <c r="R7" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
       <c r="U7" s="1">
         <v>500</v>
       </c>
@@ -1077,10 +1077,10 @@
       <c r="Y7" s="1">
         <v>4</v>
       </c>
-      <c r="Z7" s="22" t="s">
+      <c r="Z7" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="AA7" s="22"/>
+      <c r="AA7" s="21"/>
       <c r="AB7" s="13">
         <v>5</v>
       </c>
@@ -1095,32 +1095,32 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="A8" s="21">
         <v>5</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="I8" s="22">
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="I8" s="21">
         <v>5</v>
       </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22" t="s">
+      <c r="J8" s="21"/>
+      <c r="K8" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="22"/>
+      <c r="L8" s="21"/>
       <c r="Q8" s="1">
         <v>5</v>
       </c>
-      <c r="R8" s="22" t="s">
+      <c r="R8" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="S8" s="22"/>
-      <c r="T8" s="22"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
       <c r="U8" s="1">
         <v>600</v>
       </c>
@@ -1130,10 +1130,10 @@
       <c r="Y8" s="1">
         <v>5</v>
       </c>
-      <c r="Z8" s="22" t="s">
+      <c r="Z8" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="AA8" s="22"/>
+      <c r="AA8" s="21"/>
       <c r="AB8" s="13">
         <v>1</v>
       </c>
@@ -1148,106 +1148,106 @@
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="22"/>
-      <c r="AA9" s="22"/>
+      <c r="Z9" s="21"/>
+      <c r="AA9" s="21"/>
       <c r="AB9" s="13"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
       <c r="H14" s="15"/>
-      <c r="I14" s="29" t="s">
+      <c r="I14" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="Q14" s="28" t="s">
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="Q14" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="R14" s="28"/>
-      <c r="S14" s="28"/>
-      <c r="T14" s="28"/>
-      <c r="U14" s="28"/>
-      <c r="V14" s="28"/>
-      <c r="Y14" s="26" t="s">
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="Y14" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="Z14" s="26"/>
-      <c r="AA14" s="26"/>
-      <c r="AB14" s="26"/>
-      <c r="AC14" s="26"/>
-      <c r="AD14" s="26"/>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="24"/>
+      <c r="AD14" s="24"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="V15" s="28"/>
-      <c r="Y15" s="26"/>
-      <c r="Z15" s="26"/>
-      <c r="AA15" s="26"/>
-      <c r="AB15" s="26"/>
-      <c r="AC15" s="26"/>
-      <c r="AD15" s="26"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
+      <c r="Y15" s="24"/>
+      <c r="Z15" s="24"/>
+      <c r="AA15" s="24"/>
+      <c r="AB15" s="24"/>
+      <c r="AC15" s="24"/>
+      <c r="AD15" s="24"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22" t="s">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
       <c r="H16" s="15"/>
       <c r="I16" s="14" t="s">
         <v>0</v>
@@ -1264,11 +1264,11 @@
       <c r="Q16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R16" s="22" t="s">
+      <c r="R16" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
       <c r="U16" s="4" t="s">
         <v>11</v>
       </c>
@@ -1287,10 +1287,10 @@
       <c r="AB16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AC16" s="22" t="s">
+      <c r="AC16" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="AD16" s="22"/>
+      <c r="AD16" s="21"/>
       <c r="AE16" t="s">
         <v>54</v>
       </c>
@@ -1299,16 +1299,16 @@
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
+      <c r="A17" s="21">
         <v>1</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22" t="s">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
       <c r="I17" s="14">
         <v>1</v>
       </c>
@@ -1324,11 +1324,11 @@
       <c r="Q17" s="1">
         <v>1</v>
       </c>
-      <c r="R17" s="22" t="s">
+      <c r="R17" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
       <c r="U17" s="5">
         <v>5</v>
       </c>
@@ -1347,10 +1347,10 @@
       <c r="AB17" s="5">
         <v>4</v>
       </c>
-      <c r="AC17" s="22">
+      <c r="AC17" s="21">
         <v>300</v>
       </c>
-      <c r="AD17" s="22"/>
+      <c r="AD17" s="21"/>
       <c r="AE17" t="s">
         <v>56</v>
       </c>
@@ -1359,16 +1359,16 @@
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
+      <c r="A18" s="21">
         <v>2</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
       <c r="I18" s="14">
         <v>2</v>
       </c>
@@ -1384,17 +1384,17 @@
       <c r="Q18" s="1">
         <v>2</v>
       </c>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
       <c r="U18" s="5"/>
       <c r="V18" s="11"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="9"/>
       <c r="AA18" s="7"/>
       <c r="AB18" s="5"/>
-      <c r="AC18" s="22"/>
-      <c r="AD18" s="22"/>
+      <c r="AC18" s="21"/>
+      <c r="AD18" s="21"/>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I19" s="14"/>
@@ -1404,17 +1404,17 @@
       <c r="Q19" s="1">
         <v>3</v>
       </c>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
       <c r="U19" s="5"/>
       <c r="V19" s="11"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="9"/>
       <c r="AA19" s="7"/>
       <c r="AB19" s="5"/>
-      <c r="AC19" s="22"/>
-      <c r="AD19" s="22"/>
+      <c r="AC19" s="21"/>
+      <c r="AD19" s="21"/>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I20" s="14"/>
@@ -1424,24 +1424,24 @@
       <c r="Q20" s="1">
         <v>4</v>
       </c>
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="22"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
       <c r="U20" s="5"/>
       <c r="V20" s="11"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="9"/>
       <c r="AA20" s="7"/>
       <c r="AB20" s="5"/>
-      <c r="AC20" s="22"/>
-      <c r="AD20" s="22"/>
+      <c r="AC20" s="21"/>
+      <c r="AD20" s="21"/>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -1450,22 +1450,22 @@
       <c r="K21" s="18"/>
       <c r="L21" s="14"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="22"/>
-      <c r="S21" s="22"/>
-      <c r="T21" s="22"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
       <c r="U21" s="5"/>
       <c r="V21" s="11"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="9"/>
       <c r="AA21" s="7"/>
       <c r="AB21" s="5"/>
-      <c r="AC21" s="22"/>
-      <c r="AD21" s="22"/>
+      <c r="AC21" s="21"/>
+      <c r="AD21" s="21"/>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
@@ -1474,17 +1474,17 @@
       <c r="K22" s="18"/>
       <c r="L22" s="14"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="22"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
       <c r="U22" s="5"/>
       <c r="V22" s="11"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="9"/>
       <c r="AA22" s="7"/>
       <c r="AB22" s="5"/>
-      <c r="AC22" s="22"/>
-      <c r="AD22" s="22"/>
+      <c r="AC22" s="21"/>
+      <c r="AD22" s="21"/>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1501,17 +1501,17 @@
       <c r="K23" s="18"/>
       <c r="L23" s="14"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
-      <c r="T23" s="22"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
       <c r="U23" s="5"/>
       <c r="V23" s="11"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="9"/>
       <c r="AA23" s="7"/>
       <c r="AB23" s="5"/>
-      <c r="AC23" s="22"/>
-      <c r="AD23" s="22"/>
+      <c r="AC23" s="21"/>
+      <c r="AD23" s="21"/>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
@@ -1539,33 +1539,39 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="A21:C22"/>
-    <mergeCell ref="Q14:V15"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="I14:L15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A14:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="AC22:AD22"/>
-    <mergeCell ref="AC23:AD23"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="AC20:AD20"/>
-    <mergeCell ref="AC21:AD21"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="Y14:AD15"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AC18:AD18"/>
-    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="Y1:AE2"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="I1:O2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="Q1:V2"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D8:F8"/>
     <mergeCell ref="R8:T8"/>
     <mergeCell ref="R9:T9"/>
     <mergeCell ref="Z3:AA3"/>
@@ -1580,39 +1586,33 @@
     <mergeCell ref="R5:T5"/>
     <mergeCell ref="R6:T6"/>
     <mergeCell ref="R7:T7"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="Y1:AE2"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="I1:O2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="Q1:V2"/>
+    <mergeCell ref="Y14:AD15"/>
+    <mergeCell ref="AC16:AD16"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="AC20:AD20"/>
+    <mergeCell ref="AC21:AD21"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="AC22:AD22"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="A21:C22"/>
+    <mergeCell ref="Q14:V15"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="I14:L15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A14:G15"/>
+    <mergeCell ref="D16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>